<commit_message>
Modifica descrizione comportamento per timeout
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#200000SWHMEDIWARE/MEDIWARE/ADVMEDNET/2.2.1/report-checklist.xlsx
+++ b/GATEWAY/A1#200000SWHMEDIWARE/MEDIWARE/ADVMEDNET/2.2.1/report-checklist.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\angel\Google Drive\Mediware\ScambioFile\FSE2.0\Accreditamento\da inviare\A1#200000SWHMEDIWARE\MEDIWARE\ADVMEDNET\2.2.1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\angel\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06DE7478-4E93-4E92-A7BD-884A33185D87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC73B590-74CB-4158-9B4D-E6C2D36BB2DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4574,10 +4574,10 @@
     <t>2024-02-11T16:20:35Z</t>
   </si>
   <si>
-    <t>Al medico compare una finestra bloccante con il messaggio di errore ed il solo tasto OK. Il programma non esegue l'invio ed il medico può eventualmente ritentare l'invio</t>
-  </si>
-  <si>
     <t>Invio Profilo Sanitario Sintetico fallito: il server non ha risposto nel tempo previsto (timeout)</t>
+  </si>
+  <si>
+    <t>Al medico compare una finestra bloccante con il messaggio di errore, l'informazione che può ritentare l'invio e che se il problema persiste deve riprovare l'invio in un altro momento ed il solo tasto OK. Il programma non esegue l'invio ed il medico può eventualmente ritentare l'invio</t>
   </si>
 </sst>
 </file>
@@ -4914,7 +4914,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -5022,9 +5022,6 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -5040,8 +5037,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -7503,10 +7500,10 @@
   <dimension ref="A1:T1000"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="H10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="I45" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="M45" sqref="M45"/>
+      <selection pane="bottomRight" activeCell="P177" sqref="P177"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -7526,7 +7523,7 @@
     <col min="13" max="13" width="36.85546875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="33.140625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="33.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="28.28515625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="33.28515625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="12.140625" bestFit="1" customWidth="1"/>
@@ -7580,8 +7577,8 @@
       <c r="A3" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="42"/>
-      <c r="C3" s="41" t="s">
+      <c r="B3" s="41"/>
+      <c r="C3" s="46" t="s">
         <v>830</v>
       </c>
       <c r="D3" s="37"/>
@@ -7602,9 +7599,9 @@
       <c r="T3" s="15"/>
     </row>
     <row r="4" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A4" s="43"/>
-      <c r="B4" s="44"/>
-      <c r="C4" s="41" t="s">
+      <c r="A4" s="42"/>
+      <c r="B4" s="43"/>
+      <c r="C4" s="46" t="s">
         <v>829</v>
       </c>
       <c r="D4" s="37"/>
@@ -7626,9 +7623,9 @@
       <c r="T4" s="15"/>
     </row>
     <row r="5" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A5" s="45"/>
-      <c r="B5" s="46"/>
-      <c r="C5" s="41" t="s">
+      <c r="A5" s="44"/>
+      <c r="B5" s="45"/>
+      <c r="C5" s="46" t="s">
         <v>866</v>
       </c>
       <c r="D5" s="37"/>
@@ -9241,7 +9238,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="53" spans="1:20" ht="105">
+    <row r="53" spans="1:20" ht="180">
       <c r="A53" s="20">
         <v>46</v>
       </c>
@@ -9263,20 +9260,20 @@
       <c r="I53" s="24"/>
       <c r="J53" s="25"/>
       <c r="K53" s="25"/>
-      <c r="L53" s="47" t="s">
+      <c r="L53" s="25" t="s">
         <v>138</v>
       </c>
-      <c r="M53" s="47" t="s">
+      <c r="M53" s="25" t="s">
         <v>138</v>
       </c>
-      <c r="N53" s="47" t="s">
+      <c r="N53" s="25" t="s">
+        <v>870</v>
+      </c>
+      <c r="O53" s="25" t="s">
+        <v>827</v>
+      </c>
+      <c r="P53" s="25" t="s">
         <v>871</v>
-      </c>
-      <c r="O53" s="47" t="s">
-        <v>827</v>
-      </c>
-      <c r="P53" s="47" t="s">
-        <v>870</v>
       </c>
       <c r="Q53" s="25"/>
       <c r="R53" s="26" t="s">

</xml_diff>